<commit_message>
taking new demand prices
</commit_message>
<xml_diff>
--- a/Load dataset.xlsx
+++ b/Load dataset.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28308"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28317"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="365" documentId="11_5A440047DFECBC58903F4DEA860302072BED40F4" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{38FD0E2D-5D79-414D-A2EA-3CCE25AC7D9C}"/>
+  <xr:revisionPtr revIDLastSave="384" documentId="11_5A440047DFECBC58903F4DEA860302072BED40F4" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D5080DC3-7F96-4F99-9314-3B1F5E7FB518}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="3" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Load profile" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="160">
   <si>
     <t>Hour</t>
   </si>
@@ -68,6 +68,12 @@
   </si>
   <si>
     <t>Total</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Data from (november 18th 2024): </t>
+  </si>
+  <si>
+    <t>https://andelenergi.dk/el/timeenergi/</t>
   </si>
   <si>
     <t>19.11.2024 - 23:00</t>
@@ -570,17 +576,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" xr:uid="{00000000-000B-0000-0000-000008000000}"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -1350,7 +1355,7 @@
   <dimension ref="A1:B25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1564,8 +1569,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{711E96C0-72E0-40D0-B5C5-2356C5C3C468}">
   <dimension ref="A1:M151"/>
   <sheetViews>
-    <sheetView topLeftCell="A71" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1574,6 +1579,7 @@
     <col min="2" max="2" width="12" customWidth="1"/>
     <col min="3" max="3" width="19.5703125" customWidth="1"/>
     <col min="4" max="4" width="18.85546875" customWidth="1"/>
+    <col min="7" max="7" width="29.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13">
@@ -1589,15 +1595,19 @@
       <c r="D1" s="2" t="s">
         <v>9</v>
       </c>
+      <c r="G1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>11</v>
+      </c>
       <c r="J1" s="2"/>
       <c r="K1" s="2"/>
-      <c r="M1" s="2" t="s">
-        <v>9</v>
-      </c>
+      <c r="M1" s="2"/>
     </row>
     <row r="2" spans="1:13">
       <c r="A2" s="2" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B2" s="2">
         <v>1</v>
@@ -1611,7 +1621,7 @@
     </row>
     <row r="3" spans="1:13">
       <c r="A3" s="2" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B3" s="2">
         <v>1.1399999999999999</v>
@@ -1625,7 +1635,7 @@
     </row>
     <row r="4" spans="1:13">
       <c r="A4" s="2" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B4" s="2">
         <v>1.18</v>
@@ -1639,7 +1649,7 @@
     </row>
     <row r="5" spans="1:13">
       <c r="A5" s="2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B5" s="2">
         <v>1.25</v>
@@ -1653,7 +1663,7 @@
     </row>
     <row r="6" spans="1:13">
       <c r="A6" s="2" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B6" s="2">
         <v>1.33</v>
@@ -1667,7 +1677,7 @@
     </row>
     <row r="7" spans="1:13">
       <c r="A7" s="2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B7" s="2">
         <v>1.4</v>
@@ -1681,7 +1691,7 @@
     </row>
     <row r="8" spans="1:13">
       <c r="A8" s="2" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B8" s="2">
         <v>1.48</v>
@@ -1695,7 +1705,7 @@
     </row>
     <row r="9" spans="1:13">
       <c r="A9" s="2" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B9" s="2">
         <v>1.4</v>
@@ -1709,7 +1719,7 @@
     </row>
     <row r="10" spans="1:13">
       <c r="A10" s="2" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B10" s="2">
         <v>1.38</v>
@@ -1723,7 +1733,7 @@
     </row>
     <row r="11" spans="1:13">
       <c r="A11" s="2" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B11" s="2">
         <v>1.47</v>
@@ -1737,7 +1747,7 @@
     </row>
     <row r="12" spans="1:13">
       <c r="A12" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B12" s="2">
         <v>1.51</v>
@@ -1751,7 +1761,7 @@
     </row>
     <row r="13" spans="1:13">
       <c r="A13" s="2" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B13" s="2">
         <v>1.54</v>
@@ -1765,7 +1775,7 @@
     </row>
     <row r="14" spans="1:13">
       <c r="A14" s="2" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B14" s="2">
         <v>1.58</v>
@@ -1779,7 +1789,7 @@
     </row>
     <row r="15" spans="1:13">
       <c r="A15" s="2" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B15" s="2">
         <v>1.62</v>
@@ -1793,7 +1803,7 @@
     </row>
     <row r="16" spans="1:13">
       <c r="A16" s="2" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B16" s="2">
         <v>1.64</v>
@@ -1807,7 +1817,7 @@
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="2" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B17" s="2">
         <v>1.62</v>
@@ -1821,7 +1831,7 @@
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B18" s="2">
         <v>1.42</v>
@@ -1835,7 +1845,7 @@
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B19" s="2">
         <v>1.26</v>
@@ -1849,7 +1859,7 @@
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B20" s="2">
         <v>1.05</v>
@@ -1863,7 +1873,7 @@
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="2" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B21" s="2">
         <v>1.05</v>
@@ -1877,7 +1887,7 @@
     </row>
     <row r="22" spans="1:4">
       <c r="A22" s="2" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B22" s="2">
         <v>1.01</v>
@@ -1891,7 +1901,7 @@
     </row>
     <row r="23" spans="1:4">
       <c r="A23" s="2" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B23" s="2">
         <v>1.05</v>
@@ -1905,7 +1915,7 @@
     </row>
     <row r="24" spans="1:4">
       <c r="A24" s="2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B24" s="2">
         <v>1.1000000000000001</v>
@@ -1919,7 +1929,7 @@
     </row>
     <row r="25" spans="1:4">
       <c r="A25" s="2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B25" s="2">
         <v>1.1599999999999999</v>
@@ -1933,7 +1943,7 @@
     </row>
     <row r="26" spans="1:4">
       <c r="A26" s="2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B26" s="2">
         <v>1.17</v>
@@ -1947,7 +1957,7 @@
     </row>
     <row r="27" spans="1:4">
       <c r="A27" s="2" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B27" s="2">
         <v>1.25</v>
@@ -1961,7 +1971,7 @@
     </row>
     <row r="28" spans="1:4">
       <c r="A28" s="2" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B28" s="2">
         <v>1.26</v>
@@ -1975,7 +1985,7 @@
     </row>
     <row r="29" spans="1:4">
       <c r="A29" s="2" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B29" s="2">
         <v>1.35</v>
@@ -1989,7 +1999,7 @@
     </row>
     <row r="30" spans="1:4">
       <c r="A30" s="2" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B30" s="2">
         <v>1.57</v>
@@ -2003,7 +2013,7 @@
     </row>
     <row r="31" spans="1:4">
       <c r="A31" s="2" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B31" s="2">
         <v>1.67</v>
@@ -2017,7 +2027,7 @@
     </row>
     <row r="32" spans="1:4">
       <c r="A32" s="2" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B32" s="2">
         <v>1.64</v>
@@ -2031,7 +2041,7 @@
     </row>
     <row r="33" spans="1:4">
       <c r="A33" s="2" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B33" s="2">
         <v>1.38</v>
@@ -2045,7 +2055,7 @@
     </row>
     <row r="34" spans="1:4">
       <c r="A34" s="2" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B34" s="2">
         <v>1.22</v>
@@ -2059,7 +2069,7 @@
     </row>
     <row r="35" spans="1:4">
       <c r="A35" s="2" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B35" s="2">
         <v>0.93</v>
@@ -2073,7 +2083,7 @@
     </row>
     <row r="36" spans="1:4">
       <c r="A36" s="2" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B36" s="2">
         <v>0.81</v>
@@ -2087,7 +2097,7 @@
     </row>
     <row r="37" spans="1:4">
       <c r="A37" s="2" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B37" s="2">
         <v>0.88</v>
@@ -2101,7 +2111,7 @@
     </row>
     <row r="38" spans="1:4">
       <c r="A38" s="2" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B38" s="2">
         <v>0.92</v>
@@ -2115,7 +2125,7 @@
     </row>
     <row r="39" spans="1:4">
       <c r="A39" s="2" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B39" s="2">
         <v>0.96</v>
@@ -2129,7 +2139,7 @@
     </row>
     <row r="40" spans="1:4">
       <c r="A40" s="2" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B40" s="2">
         <v>1.1100000000000001</v>
@@ -2143,7 +2153,7 @@
     </row>
     <row r="41" spans="1:4">
       <c r="A41" s="2" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B41" s="2">
         <v>1.26</v>
@@ -2157,7 +2167,7 @@
     </row>
     <row r="42" spans="1:4">
       <c r="A42" s="2" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B42" s="2">
         <v>1.0900000000000001</v>
@@ -2171,7 +2181,7 @@
     </row>
     <row r="43" spans="1:4">
       <c r="A43" s="2" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B43" s="2">
         <v>0.74</v>
@@ -2185,7 +2195,7 @@
     </row>
     <row r="44" spans="1:4">
       <c r="A44" s="2" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B44" s="2">
         <v>0.44</v>
@@ -2199,7 +2209,7 @@
     </row>
     <row r="45" spans="1:4">
       <c r="A45" s="2" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B45" s="2">
         <v>0.4</v>
@@ -2213,7 +2223,7 @@
     </row>
     <row r="46" spans="1:4">
       <c r="A46" s="2" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B46" s="2">
         <v>0.28999999999999998</v>
@@ -2227,7 +2237,7 @@
     </row>
     <row r="47" spans="1:4">
       <c r="A47" s="2" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B47" s="2">
         <v>0.28999999999999998</v>
@@ -2241,7 +2251,7 @@
     </row>
     <row r="48" spans="1:4">
       <c r="A48" s="2" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B48" s="2">
         <v>0.28000000000000003</v>
@@ -2255,7 +2265,7 @@
     </row>
     <row r="49" spans="1:4">
       <c r="A49" s="2" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B49" s="2">
         <v>0.28000000000000003</v>
@@ -2269,7 +2279,7 @@
     </row>
     <row r="50" spans="1:4">
       <c r="A50" s="2" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B50" s="2">
         <v>0.38</v>
@@ -2283,7 +2293,7 @@
     </row>
     <row r="51" spans="1:4">
       <c r="A51" s="2" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B51" s="2">
         <v>0.45</v>
@@ -2297,7 +2307,7 @@
     </row>
     <row r="52" spans="1:4">
       <c r="A52" s="2" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B52" s="2">
         <v>0.49</v>
@@ -2311,7 +2321,7 @@
     </row>
     <row r="53" spans="1:4">
       <c r="A53" s="2" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B53" s="2">
         <v>0.5</v>
@@ -2325,7 +2335,7 @@
     </row>
     <row r="54" spans="1:4">
       <c r="A54" s="2" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B54" s="2">
         <v>0.51</v>
@@ -2339,7 +2349,7 @@
     </row>
     <row r="55" spans="1:4">
       <c r="A55" s="2" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B55" s="2">
         <v>0.52</v>
@@ -2353,7 +2363,7 @@
     </row>
     <row r="56" spans="1:4">
       <c r="A56" s="2" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B56" s="2">
         <v>0.53</v>
@@ -2367,7 +2377,7 @@
     </row>
     <row r="57" spans="1:4">
       <c r="A57" s="2" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B57" s="2">
         <v>0.52</v>
@@ -2381,7 +2391,7 @@
     </row>
     <row r="58" spans="1:4">
       <c r="A58" s="2" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B58" s="2">
         <v>0.47</v>
@@ -2395,7 +2405,7 @@
     </row>
     <row r="59" spans="1:4">
       <c r="A59" s="2" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B59" s="2">
         <v>0.51</v>
@@ -2409,7 +2419,7 @@
     </row>
     <row r="60" spans="1:4">
       <c r="A60" s="2" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B60" s="2">
         <v>0.3</v>
@@ -2423,7 +2433,7 @@
     </row>
     <row r="61" spans="1:4">
       <c r="A61" s="2" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B61" s="2">
         <v>0.34</v>
@@ -2437,7 +2447,7 @@
     </row>
     <row r="62" spans="1:4">
       <c r="A62" s="2" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B62" s="2">
         <v>0.34</v>
@@ -2451,7 +2461,7 @@
     </row>
     <row r="63" spans="1:4">
       <c r="A63" s="2" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B63" s="2">
         <v>0.38</v>
@@ -2465,7 +2475,7 @@
     </row>
     <row r="64" spans="1:4">
       <c r="A64" s="2" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B64" s="2">
         <v>0.44</v>
@@ -2479,7 +2489,7 @@
     </row>
     <row r="65" spans="1:4">
       <c r="A65" s="2" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B65" s="2">
         <v>0.43</v>
@@ -2493,7 +2503,7 @@
     </row>
     <row r="66" spans="1:4">
       <c r="A66" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B66" s="2">
         <v>0.45</v>
@@ -2507,7 +2517,7 @@
     </row>
     <row r="67" spans="1:4">
       <c r="A67" s="2" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B67" s="2">
         <v>0.41</v>
@@ -2521,7 +2531,7 @@
     </row>
     <row r="68" spans="1:4">
       <c r="A68" s="2" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B68" s="2">
         <v>0.35</v>
@@ -2535,7 +2545,7 @@
     </row>
     <row r="69" spans="1:4">
       <c r="A69" s="2" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B69" s="2">
         <v>0.39</v>
@@ -2549,7 +2559,7 @@
     </row>
     <row r="70" spans="1:4">
       <c r="A70" s="2" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="B70" s="2">
         <v>0.43</v>
@@ -2563,7 +2573,7 @@
     </row>
     <row r="71" spans="1:4">
       <c r="A71" s="2" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B71" s="2">
         <v>0.44</v>
@@ -2577,7 +2587,7 @@
     </row>
     <row r="72" spans="1:4">
       <c r="A72" s="2" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B72" s="2">
         <v>0.37</v>
@@ -2591,7 +2601,7 @@
     </row>
     <row r="73" spans="1:4">
       <c r="A73" s="2" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B73" s="2">
         <v>0.31</v>
@@ -2605,7 +2615,7 @@
     </row>
     <row r="74" spans="1:4">
       <c r="A74" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B74" s="2">
         <v>0.41</v>
@@ -2619,7 +2629,7 @@
     </row>
     <row r="75" spans="1:4">
       <c r="A75" s="2" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="B75" s="2">
         <v>0.47</v>
@@ -2633,7 +2643,7 @@
     </row>
     <row r="76" spans="1:4">
       <c r="A76" s="2" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="B76" s="2">
         <v>0.52</v>
@@ -2647,7 +2657,7 @@
     </row>
     <row r="77" spans="1:4">
       <c r="A77" s="2" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B77" s="2">
         <v>0.5</v>
@@ -2661,7 +2671,7 @@
     </row>
     <row r="78" spans="1:4">
       <c r="A78" s="2" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="B78" s="2">
         <v>0.53</v>
@@ -2675,7 +2685,7 @@
     </row>
     <row r="79" spans="1:4">
       <c r="A79" s="2" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B79" s="2">
         <v>0.57999999999999996</v>
@@ -2689,7 +2699,7 @@
     </row>
     <row r="80" spans="1:4">
       <c r="A80" s="2" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="B80" s="2">
         <v>0.6</v>
@@ -2703,7 +2713,7 @@
     </row>
     <row r="81" spans="1:4">
       <c r="A81" s="2" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B81" s="2">
         <v>0.52</v>
@@ -2717,7 +2727,7 @@
     </row>
     <row r="82" spans="1:4">
       <c r="A82" s="2" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="B82" s="2">
         <v>0.5</v>
@@ -2731,7 +2741,7 @@
     </row>
     <row r="83" spans="1:4">
       <c r="A83" s="2" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="B83" s="2">
         <v>0.43</v>
@@ -2745,7 +2755,7 @@
     </row>
     <row r="84" spans="1:4">
       <c r="A84" s="2" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B84" s="2">
         <v>0.41</v>
@@ -2759,7 +2769,7 @@
     </row>
     <row r="85" spans="1:4">
       <c r="A85" s="2" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="B85" s="2">
         <v>0.42</v>
@@ -2773,7 +2783,7 @@
     </row>
     <row r="86" spans="1:4">
       <c r="A86" s="2" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="B86" s="2">
         <v>0.41</v>
@@ -2787,7 +2797,7 @@
     </row>
     <row r="87" spans="1:4">
       <c r="A87" s="2" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B87" s="2">
         <v>0.37</v>
@@ -2801,7 +2811,7 @@
     </row>
     <row r="88" spans="1:4">
       <c r="A88" s="2" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="B88" s="2">
         <v>0.27</v>
@@ -2815,7 +2825,7 @@
     </row>
     <row r="89" spans="1:4">
       <c r="A89" s="2" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="B89" s="2">
         <v>0.26</v>
@@ -2829,7 +2839,7 @@
     </row>
     <row r="90" spans="1:4">
       <c r="A90" s="2" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="B90" s="2">
         <v>0.19</v>
@@ -2843,7 +2853,7 @@
     </row>
     <row r="91" spans="1:4">
       <c r="A91" s="2" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B91" s="2">
         <v>0.19</v>
@@ -2857,7 +2867,7 @@
     </row>
     <row r="92" spans="1:4">
       <c r="A92" s="2" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="B92" s="2">
         <v>0.19</v>
@@ -2871,7 +2881,7 @@
     </row>
     <row r="93" spans="1:4">
       <c r="A93" s="2" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B93" s="2">
         <v>0.19</v>
@@ -2885,7 +2895,7 @@
     </row>
     <row r="94" spans="1:4">
       <c r="A94" s="2" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="B94" s="2">
         <v>0.19</v>
@@ -2899,7 +2909,7 @@
     </row>
     <row r="95" spans="1:4">
       <c r="A95" s="2" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="B95" s="2">
         <v>0.19</v>
@@ -2913,7 +2923,7 @@
     </row>
     <row r="96" spans="1:4">
       <c r="A96" s="2" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="B96" s="2">
         <v>0.25</v>
@@ -2927,7 +2937,7 @@
     </row>
     <row r="97" spans="1:4">
       <c r="A97" s="2" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="B97" s="2">
         <v>0.27</v>
@@ -2941,7 +2951,7 @@
     </row>
     <row r="98" spans="1:4">
       <c r="A98" s="2" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="B98" s="2">
         <v>0.27</v>
@@ -2955,7 +2965,7 @@
     </row>
     <row r="99" spans="1:4">
       <c r="A99" s="2" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="B99" s="2">
         <v>0.31</v>
@@ -2969,7 +2979,7 @@
     </row>
     <row r="100" spans="1:4">
       <c r="A100" s="2" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="B100" s="2">
         <v>0.46</v>
@@ -2983,7 +2993,7 @@
     </row>
     <row r="101" spans="1:4">
       <c r="A101" s="2" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="B101" s="2">
         <v>0.53</v>
@@ -2997,7 +3007,7 @@
     </row>
     <row r="102" spans="1:4">
       <c r="A102" s="2" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="B102" s="2">
         <v>0.53</v>
@@ -3011,7 +3021,7 @@
     </row>
     <row r="103" spans="1:4">
       <c r="A103" s="2" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="B103" s="2">
         <v>0.87</v>
@@ -3025,7 +3035,7 @@
     </row>
     <row r="104" spans="1:4">
       <c r="A104" s="2" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="B104" s="2">
         <v>1.0900000000000001</v>
@@ -3039,7 +3049,7 @@
     </row>
     <row r="105" spans="1:4">
       <c r="A105" s="2" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="B105" s="2">
         <v>1.05</v>
@@ -3053,7 +3063,7 @@
     </row>
     <row r="106" spans="1:4">
       <c r="A106" s="2" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="B106" s="2">
         <v>1.04</v>
@@ -3067,7 +3077,7 @@
     </row>
     <row r="107" spans="1:4">
       <c r="A107" s="2" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="B107" s="2">
         <v>1.04</v>
@@ -3081,7 +3091,7 @@
     </row>
     <row r="108" spans="1:4">
       <c r="A108" s="2" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="B108" s="2">
         <v>1.06</v>
@@ -3095,7 +3105,7 @@
     </row>
     <row r="109" spans="1:4">
       <c r="A109" s="2" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="B109" s="2">
         <v>1.1100000000000001</v>
@@ -3109,7 +3119,7 @@
     </row>
     <row r="110" spans="1:4">
       <c r="A110" s="2" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="B110" s="2">
         <v>1.1599999999999999</v>
@@ -3123,7 +3133,7 @@
     </row>
     <row r="111" spans="1:4">
       <c r="A111" s="2" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="B111" s="2">
         <v>1.41</v>
@@ -3137,7 +3147,7 @@
     </row>
     <row r="112" spans="1:4">
       <c r="A112" s="2" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="B112" s="2">
         <v>1.44</v>
@@ -3151,7 +3161,7 @@
     </row>
     <row r="113" spans="1:4">
       <c r="A113" s="2" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B113" s="2">
         <v>1.53</v>
@@ -3165,7 +3175,7 @@
     </row>
     <row r="114" spans="1:4">
       <c r="A114" s="2" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="B114" s="2">
         <v>1.35</v>
@@ -3179,7 +3189,7 @@
     </row>
     <row r="115" spans="1:4">
       <c r="A115" s="2" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="B115" s="2">
         <v>1.04</v>
@@ -3193,7 +3203,7 @@
     </row>
     <row r="116" spans="1:4">
       <c r="A116" s="2" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="B116" s="2">
         <v>0.99</v>
@@ -3207,7 +3217,7 @@
     </row>
     <row r="117" spans="1:4">
       <c r="A117" s="2" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="B117" s="2">
         <v>0.99</v>
@@ -3221,7 +3231,7 @@
     </row>
     <row r="118" spans="1:4">
       <c r="A118" s="2" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B118" s="2">
         <v>1.0900000000000001</v>
@@ -3235,7 +3245,7 @@
     </row>
     <row r="119" spans="1:4">
       <c r="A119" s="2" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="B119" s="2">
         <v>1.0900000000000001</v>
@@ -3249,7 +3259,7 @@
     </row>
     <row r="120" spans="1:4">
       <c r="A120" s="2" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="B120" s="2">
         <v>1.1100000000000001</v>
@@ -3263,7 +3273,7 @@
     </row>
     <row r="121" spans="1:4">
       <c r="A121" s="2" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="B121" s="2">
         <v>1.1299999999999999</v>
@@ -3277,7 +3287,7 @@
     </row>
     <row r="122" spans="1:4">
       <c r="A122" s="2" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="B122" s="2">
         <v>1.21</v>
@@ -3291,7 +3301,7 @@
     </row>
     <row r="123" spans="1:4">
       <c r="A123" s="2" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="B123" s="2">
         <v>1.3</v>
@@ -3305,7 +3315,7 @@
     </row>
     <row r="124" spans="1:4">
       <c r="A124" s="2" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="B124" s="2">
         <v>1.37</v>
@@ -3319,7 +3329,7 @@
     </row>
     <row r="125" spans="1:4">
       <c r="A125" s="2" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="B125" s="2">
         <v>1.45</v>
@@ -3333,7 +3343,7 @@
     </row>
     <row r="126" spans="1:4">
       <c r="A126" s="2" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="B126" s="2">
         <v>1.54</v>
@@ -3347,7 +3357,7 @@
     </row>
     <row r="127" spans="1:4">
       <c r="A127" s="2" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="B127" s="2">
         <v>1.6</v>
@@ -3361,7 +3371,7 @@
     </row>
     <row r="128" spans="1:4">
       <c r="A128" s="2" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="B128" s="2">
         <v>1.61</v>
@@ -3375,7 +3385,7 @@
     </row>
     <row r="129" spans="1:4">
       <c r="A129" s="2" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="B129" s="2">
         <v>1.53</v>
@@ -3389,7 +3399,7 @@
     </row>
     <row r="130" spans="1:4">
       <c r="A130" s="2" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="B130" s="2">
         <v>1.48</v>
@@ -3403,7 +3413,7 @@
     </row>
     <row r="131" spans="1:4">
       <c r="A131" s="2" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="B131" s="2">
         <v>1.41</v>
@@ -3417,7 +3427,7 @@
     </row>
     <row r="132" spans="1:4">
       <c r="A132" s="2" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="B132" s="2">
         <v>1.35</v>
@@ -3431,7 +3441,7 @@
     </row>
     <row r="133" spans="1:4">
       <c r="A133" s="2" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="B133" s="2">
         <v>1.22</v>
@@ -3445,7 +3455,7 @@
     </row>
     <row r="134" spans="1:4">
       <c r="A134" s="2" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="B134" s="2">
         <v>1.2</v>
@@ -3459,7 +3469,7 @@
     </row>
     <row r="135" spans="1:4">
       <c r="A135" s="2" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="B135" s="2">
         <v>1.17</v>
@@ -3473,7 +3483,7 @@
     </row>
     <row r="136" spans="1:4">
       <c r="A136" s="2" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="B136" s="2">
         <v>1.2</v>
@@ -3487,7 +3497,7 @@
     </row>
     <row r="137" spans="1:4">
       <c r="A137" s="2" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="B137" s="2">
         <v>1.25</v>
@@ -3501,7 +3511,7 @@
     </row>
     <row r="138" spans="1:4">
       <c r="A138" s="2" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="B138" s="2">
         <v>1.1000000000000001</v>
@@ -3515,7 +3525,7 @@
     </row>
     <row r="139" spans="1:4">
       <c r="A139" s="2" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="B139" s="2">
         <v>0.92</v>
@@ -3529,7 +3539,7 @@
     </row>
     <row r="140" spans="1:4">
       <c r="A140" s="2" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="B140" s="2">
         <v>0.63</v>
@@ -3543,7 +3553,7 @@
     </row>
     <row r="141" spans="1:4">
       <c r="A141" s="2" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="B141" s="2">
         <v>0.56000000000000005</v>
@@ -3557,7 +3567,7 @@
     </row>
     <row r="142" spans="1:4">
       <c r="A142" s="2" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="B142" s="2">
         <v>0.62</v>
@@ -3571,7 +3581,7 @@
     </row>
     <row r="143" spans="1:4">
       <c r="A143" s="2" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="B143" s="2">
         <v>0.61</v>
@@ -3585,7 +3595,7 @@
     </row>
     <row r="144" spans="1:4">
       <c r="A144" s="2" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="B144" s="2">
         <v>0.61</v>
@@ -3599,7 +3609,7 @@
     </row>
     <row r="145" spans="1:4">
       <c r="A145" s="2" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="B145" s="2">
         <v>0.64</v>
@@ -3643,6 +3653,9 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:D145" xr:uid="{711E96C0-72E0-40D0-B5C5-2356C5C3C468}"/>
+  <hyperlinks>
+    <hyperlink ref="H1" r:id="rId1" xr:uid="{B7E78482-F2B8-495B-B18E-FCD1220C6932}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -3652,7 +3665,7 @@
   <dimension ref="A2:L168"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q18" sqref="Q18"/>
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3676,41 +3689,41 @@
         <v>9</v>
       </c>
       <c r="I2" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="J2">
         <v>0.14169615999999999</v>
       </c>
       <c r="K2" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
     </row>
     <row r="3" spans="1:12">
       <c r="A3" s="2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B3" s="2">
         <v>1.1599999999999999</v>
       </c>
       <c r="C3" s="2">
-        <v>1.25</v>
+        <v>0</v>
       </c>
       <c r="D3" s="2">
         <v>2.41</v>
       </c>
-      <c r="J3" s="5" t="s">
-        <v>156</v>
+      <c r="J3" s="4" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="4" spans="1:12">
       <c r="A4" s="2" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B4" s="2">
         <v>0.28000000000000003</v>
       </c>
       <c r="C4" s="2">
-        <v>1.25</v>
+        <v>0</v>
       </c>
       <c r="D4" s="2">
         <v>1.53</v>
@@ -3718,13 +3731,13 @@
     </row>
     <row r="5" spans="1:12">
       <c r="A5" s="2" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B5" s="2">
         <v>0.31</v>
       </c>
       <c r="C5" s="2">
-        <v>1.25</v>
+        <v>0</v>
       </c>
       <c r="D5" s="2">
         <v>1.56</v>
@@ -3733,7 +3746,7 @@
         <v>0</v>
       </c>
       <c r="J5" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="K5" t="s">
         <v>5</v>
@@ -3742,13 +3755,13 @@
     </row>
     <row r="6" spans="1:12">
       <c r="A6" s="2" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="B6" s="2">
         <v>0.27</v>
       </c>
       <c r="C6" s="2">
-        <v>1.25</v>
+        <v>0</v>
       </c>
       <c r="D6" s="2">
         <v>1.52</v>
@@ -3757,22 +3770,23 @@
         <v>1</v>
       </c>
       <c r="J6">
-        <v>1.8699999999999999</v>
+        <f>B9</f>
+        <v>0.63166666666666671</v>
       </c>
       <c r="K6">
         <f>J6*$J$2/1000</f>
-        <v>2.6497181919999996E-4</v>
+        <v>8.9504741066666666E-5</v>
       </c>
     </row>
     <row r="7" spans="1:12">
       <c r="A7" s="2" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="B7" s="2">
         <v>1.1299999999999999</v>
       </c>
       <c r="C7" s="2">
-        <v>1.25</v>
+        <v>0</v>
       </c>
       <c r="D7" s="2">
         <v>2.38</v>
@@ -3780,23 +3794,24 @@
       <c r="I7">
         <v>2</v>
       </c>
-      <c r="J7" s="4">
-        <v>1.8616666666666664</v>
+      <c r="J7">
+        <f>B16</f>
+        <v>0.62</v>
       </c>
       <c r="K7">
         <f t="shared" ref="K7:K29" si="0">J7*$J$2/1000</f>
-        <v>2.6379101786666657E-4</v>
+        <v>8.7851619199999999E-5</v>
       </c>
     </row>
     <row r="8" spans="1:12">
       <c r="A8" s="2" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="B8" s="2">
         <v>0.64</v>
       </c>
       <c r="C8" s="2">
-        <v>1.25</v>
+        <v>0</v>
       </c>
       <c r="D8" s="2">
         <v>1.89</v>
@@ -3805,11 +3820,12 @@
         <v>3</v>
       </c>
       <c r="J8">
-        <v>1.8549999999999998</v>
+        <f>B23</f>
+        <v>0.61166666666666669</v>
       </c>
       <c r="K8">
         <f t="shared" si="0"/>
-        <v>2.6284637679999996E-4</v>
+        <v>8.6670817866666666E-5</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -3817,34 +3833,34 @@
         <f>AVERAGE(B3:B8)</f>
         <v>0.63166666666666671</v>
       </c>
-      <c r="C9" s="3">
-        <f t="shared" ref="C9:D9" si="1">AVERAGE(C3:C8)</f>
-        <v>1.25</v>
+      <c r="C9" s="2">
+        <v>0</v>
       </c>
       <c r="D9" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="C9:D9" si="1">AVERAGE(D3:D8)</f>
         <v>1.8816666666666666</v>
       </c>
       <c r="I9">
         <v>4</v>
       </c>
       <c r="J9">
-        <v>1.7560000000000002</v>
+        <f>B30</f>
+        <v>0.60499999999999998</v>
       </c>
       <c r="K9">
         <f t="shared" si="0"/>
-        <v>2.4881845695999999E-4</v>
+        <v>8.5726176799999986E-5</v>
       </c>
     </row>
     <row r="10" spans="1:12">
       <c r="A10" s="2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B10" s="2">
         <v>1.1000000000000001</v>
       </c>
       <c r="C10" s="2">
-        <v>1.25</v>
+        <v>0</v>
       </c>
       <c r="D10" s="2">
         <v>2.35</v>
@@ -3862,13 +3878,13 @@
     </row>
     <row r="11" spans="1:12">
       <c r="A11" s="2" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B11" s="2">
         <v>0.28000000000000003</v>
       </c>
       <c r="C11" s="2">
-        <v>1.25</v>
+        <v>0</v>
       </c>
       <c r="D11" s="2">
         <v>1.53</v>
@@ -3886,13 +3902,13 @@
     </row>
     <row r="12" spans="1:12">
       <c r="A12" s="2" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B12" s="2">
         <v>0.37</v>
       </c>
       <c r="C12" s="2">
-        <v>1.25</v>
+        <v>0</v>
       </c>
       <c r="D12" s="2">
         <v>1.62</v>
@@ -3910,13 +3926,13 @@
     </row>
     <row r="13" spans="1:12">
       <c r="A13" s="2" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="B13" s="2">
         <v>0.25</v>
       </c>
       <c r="C13" s="2">
-        <v>1.25</v>
+        <v>0</v>
       </c>
       <c r="D13" s="2">
         <v>1.5</v>
@@ -3934,13 +3950,13 @@
     </row>
     <row r="14" spans="1:12">
       <c r="A14" s="2" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="B14" s="2">
         <v>1.1100000000000001</v>
       </c>
       <c r="C14" s="2">
-        <v>1.25</v>
+        <v>0</v>
       </c>
       <c r="D14" s="2">
         <v>2.36</v>
@@ -3958,13 +3974,13 @@
     </row>
     <row r="15" spans="1:12">
       <c r="A15" s="2" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="B15" s="2">
         <v>0.61</v>
       </c>
       <c r="C15" s="2">
-        <v>1.25</v>
+        <v>0</v>
       </c>
       <c r="D15" s="2">
         <v>1.86</v>
@@ -3985,12 +4001,11 @@
         <f>AVERAGE(B10:B15)</f>
         <v>0.62</v>
       </c>
-      <c r="C16" s="3">
-        <f t="shared" ref="C16:D16" si="2">AVERAGE(C10:C15)</f>
-        <v>1.25</v>
+      <c r="C16" s="2">
+        <v>0</v>
       </c>
       <c r="D16" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="C16:D16" si="2">AVERAGE(D10:D15)</f>
         <v>1.8699999999999999</v>
       </c>
       <c r="I16">
@@ -4006,13 +4021,13 @@
     </row>
     <row r="17" spans="1:11">
       <c r="A17" s="2" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B17" s="2">
         <v>1.05</v>
       </c>
       <c r="C17" s="2">
-        <v>1.25</v>
+        <v>0</v>
       </c>
       <c r="D17" s="2">
         <v>2.2999999999999998</v>
@@ -4030,13 +4045,13 @@
     </row>
     <row r="18" spans="1:11">
       <c r="A18" s="2" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B18" s="2">
         <v>0.28999999999999998</v>
       </c>
       <c r="C18" s="2">
-        <v>1.25</v>
+        <v>0</v>
       </c>
       <c r="D18" s="2">
         <v>1.54</v>
@@ -4054,13 +4069,13 @@
     </row>
     <row r="19" spans="1:11">
       <c r="A19" s="2" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B19" s="2">
         <v>0.44</v>
       </c>
       <c r="C19" s="2">
-        <v>1.25</v>
+        <v>0</v>
       </c>
       <c r="D19" s="2">
         <v>1.69</v>
@@ -4078,13 +4093,13 @@
     </row>
     <row r="20" spans="1:11">
       <c r="A20" s="2" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="B20" s="2">
         <v>0.19</v>
       </c>
       <c r="C20" s="2">
-        <v>1.25</v>
+        <v>0</v>
       </c>
       <c r="D20" s="2">
         <v>1.44</v>
@@ -4102,13 +4117,13 @@
     </row>
     <row r="21" spans="1:11">
       <c r="A21" s="2" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="B21" s="2">
         <v>1.0900000000000001</v>
       </c>
       <c r="C21" s="2">
-        <v>1.25</v>
+        <v>0</v>
       </c>
       <c r="D21" s="2">
         <v>2.34</v>
@@ -4126,13 +4141,13 @@
     </row>
     <row r="22" spans="1:11">
       <c r="A22" s="2" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="B22" s="2">
         <v>0.61</v>
       </c>
       <c r="C22" s="2">
-        <v>1.25</v>
+        <v>0</v>
       </c>
       <c r="D22" s="2">
         <v>1.86</v>
@@ -4153,12 +4168,11 @@
         <f>AVERAGE(B17:B22)</f>
         <v>0.61166666666666669</v>
       </c>
-      <c r="C23" s="3">
-        <f t="shared" ref="C23:D23" si="3">AVERAGE(C17:C22)</f>
-        <v>1.25</v>
+      <c r="C23" s="2">
+        <v>0</v>
       </c>
       <c r="D23" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="C23:D23" si="3">AVERAGE(D17:D22)</f>
         <v>1.8616666666666664</v>
       </c>
       <c r="I23">
@@ -4174,13 +4188,13 @@
     </row>
     <row r="24" spans="1:11">
       <c r="A24" s="2" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B24" s="2">
         <v>1.01</v>
       </c>
       <c r="C24" s="2">
-        <v>1.25</v>
+        <v>0</v>
       </c>
       <c r="D24" s="2">
         <v>2.2599999999999998</v>
@@ -4198,13 +4212,13 @@
     </row>
     <row r="25" spans="1:11">
       <c r="A25" s="2" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B25" s="2">
         <v>0.28999999999999998</v>
       </c>
       <c r="C25" s="2">
-        <v>1.25</v>
+        <v>0</v>
       </c>
       <c r="D25" s="2">
         <v>1.54</v>
@@ -4222,13 +4236,13 @@
     </row>
     <row r="26" spans="1:11">
       <c r="A26" s="2" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="B26" s="2">
         <v>0.43</v>
       </c>
       <c r="C26" s="2">
-        <v>1.25</v>
+        <v>0</v>
       </c>
       <c r="D26" s="2">
         <v>1.68</v>
@@ -4246,13 +4260,13 @@
     </row>
     <row r="27" spans="1:11">
       <c r="A27" s="2" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="B27" s="2">
         <v>0.19</v>
       </c>
       <c r="C27" s="2">
-        <v>1.25</v>
+        <v>0</v>
       </c>
       <c r="D27" s="2">
         <v>1.44</v>
@@ -4270,13 +4284,13 @@
     </row>
     <row r="28" spans="1:11">
       <c r="A28" s="2" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B28" s="2">
         <v>1.0900000000000001</v>
       </c>
       <c r="C28" s="2">
-        <v>1.25</v>
+        <v>0</v>
       </c>
       <c r="D28" s="2">
         <v>2.34</v>
@@ -4294,13 +4308,13 @@
     </row>
     <row r="29" spans="1:11">
       <c r="A29" s="2" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="B29" s="2">
         <v>0.62</v>
       </c>
       <c r="C29" s="2">
-        <v>1.25</v>
+        <v>0</v>
       </c>
       <c r="D29" s="2">
         <v>1.87</v>
@@ -4321,24 +4335,23 @@
         <f>AVERAGE(B24:B29)</f>
         <v>0.60499999999999998</v>
       </c>
-      <c r="C30" s="3">
-        <f t="shared" ref="C30:D30" si="4">AVERAGE(C24:C29)</f>
-        <v>1.25</v>
+      <c r="C30" s="2">
+        <v>0</v>
       </c>
       <c r="D30" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" ref="C30:D30" si="4">AVERAGE(D24:D29)</f>
         <v>1.8549999999999998</v>
       </c>
     </row>
     <row r="31" spans="1:11">
       <c r="A31" s="2" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B31" s="2">
         <v>0.4</v>
       </c>
       <c r="C31" s="2">
-        <v>1.25</v>
+        <v>0</v>
       </c>
       <c r="D31" s="2">
         <v>1.65</v>
@@ -4346,13 +4359,13 @@
     </row>
     <row r="32" spans="1:11">
       <c r="A32" s="2" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B32" s="2">
         <v>0.39</v>
       </c>
       <c r="C32" s="2">
-        <v>1.25</v>
+        <v>0</v>
       </c>
       <c r="D32" s="2">
         <v>1.64</v>
@@ -4360,13 +4373,13 @@
     </row>
     <row r="33" spans="1:4">
       <c r="A33" s="2" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B33" s="2">
         <v>0.19</v>
       </c>
       <c r="C33" s="2">
-        <v>1.25</v>
+        <v>0</v>
       </c>
       <c r="D33" s="2">
         <v>1.44</v>
@@ -4374,13 +4387,13 @@
     </row>
     <row r="34" spans="1:4">
       <c r="A34" s="2" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="B34" s="2">
         <v>0.99</v>
       </c>
       <c r="C34" s="2">
-        <v>1.25</v>
+        <v>0</v>
       </c>
       <c r="D34" s="2">
         <v>2.2400000000000002</v>
@@ -4388,13 +4401,13 @@
     </row>
     <row r="35" spans="1:4">
       <c r="A35" s="2" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="B35" s="2">
         <v>0.56000000000000005</v>
       </c>
       <c r="C35" s="2">
-        <v>1.25</v>
+        <v>0</v>
       </c>
       <c r="D35" s="2">
         <v>1.81</v>
@@ -4405,24 +4418,23 @@
         <f>AVERAGE(B31:B35)</f>
         <v>0.50600000000000001</v>
       </c>
-      <c r="C36" s="3">
-        <f t="shared" ref="C36:D36" si="5">AVERAGE(C31:C35)</f>
-        <v>1.25</v>
+      <c r="C36" s="2">
+        <v>0</v>
       </c>
       <c r="D36" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" ref="C36:D36" si="5">AVERAGE(D31:D35)</f>
         <v>1.7560000000000002</v>
       </c>
     </row>
     <row r="37" spans="1:4">
       <c r="A37" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B37" s="2">
         <v>1.05</v>
       </c>
       <c r="C37" s="2">
-        <v>1.25</v>
+        <v>0</v>
       </c>
       <c r="D37" s="2">
         <v>2.2999999999999998</v>
@@ -4430,13 +4442,13 @@
     </row>
     <row r="38" spans="1:4">
       <c r="A38" s="2" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B38" s="2">
         <v>0.44</v>
       </c>
       <c r="C38" s="2">
-        <v>1.25</v>
+        <v>0</v>
       </c>
       <c r="D38" s="2">
         <v>1.69</v>
@@ -4444,13 +4456,13 @@
     </row>
     <row r="39" spans="1:4">
       <c r="A39" s="2" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B39" s="2">
         <v>0.35</v>
       </c>
       <c r="C39" s="2">
-        <v>1.25</v>
+        <v>0</v>
       </c>
       <c r="D39" s="2">
         <v>1.6</v>
@@ -4458,13 +4470,13 @@
     </row>
     <row r="40" spans="1:4">
       <c r="A40" s="2" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="B40" s="2">
         <v>0.19</v>
       </c>
       <c r="C40" s="2">
-        <v>1.25</v>
+        <v>0</v>
       </c>
       <c r="D40" s="2">
         <v>1.44</v>
@@ -4472,13 +4484,13 @@
     </row>
     <row r="41" spans="1:4">
       <c r="A41" s="2" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="B41" s="2">
         <v>0.99</v>
       </c>
       <c r="C41" s="2">
-        <v>1.25</v>
+        <v>0</v>
       </c>
       <c r="D41" s="2">
         <v>2.2400000000000002</v>
@@ -4486,13 +4498,13 @@
     </row>
     <row r="42" spans="1:4">
       <c r="A42" s="2" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="B42" s="2">
         <v>0.63</v>
       </c>
       <c r="C42" s="2">
-        <v>1.25</v>
+        <v>0</v>
       </c>
       <c r="D42" s="2">
         <v>1.88</v>
@@ -4503,24 +4515,23 @@
         <f>AVERAGE(B37:B42)</f>
         <v>0.60833333333333328</v>
       </c>
-      <c r="C43" s="3">
-        <f t="shared" ref="C43:D43" si="6">AVERAGE(C37:C42)</f>
-        <v>1.25</v>
+      <c r="C43" s="2">
+        <v>0</v>
       </c>
       <c r="D43" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" ref="C43:D43" si="6">AVERAGE(D37:D42)</f>
         <v>1.8583333333333332</v>
       </c>
     </row>
     <row r="44" spans="1:4">
       <c r="A44" s="2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B44" s="2">
         <v>1.26</v>
       </c>
       <c r="C44" s="2">
-        <v>1.54</v>
+        <v>0</v>
       </c>
       <c r="D44" s="2">
         <v>2.8</v>
@@ -4528,13 +4539,13 @@
     </row>
     <row r="45" spans="1:4">
       <c r="A45" s="2" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B45" s="2">
         <v>0.74</v>
       </c>
       <c r="C45" s="2">
-        <v>1.54</v>
+        <v>0</v>
       </c>
       <c r="D45" s="2">
         <v>2.2799999999999998</v>
@@ -4542,13 +4553,13 @@
     </row>
     <row r="46" spans="1:4">
       <c r="A46" s="2" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B46" s="2">
         <v>0.41</v>
       </c>
       <c r="C46" s="2">
-        <v>1.54</v>
+        <v>0</v>
       </c>
       <c r="D46" s="2">
         <v>1.95</v>
@@ -4556,13 +4567,13 @@
     </row>
     <row r="47" spans="1:4">
       <c r="A47" s="2" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B47" s="2">
         <v>0.19</v>
       </c>
       <c r="C47" s="2">
-        <v>1.54</v>
+        <v>0</v>
       </c>
       <c r="D47" s="2">
         <v>1.73</v>
@@ -4570,13 +4581,13 @@
     </row>
     <row r="48" spans="1:4">
       <c r="A48" s="2" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="B48" s="2">
         <v>1.04</v>
       </c>
       <c r="C48" s="2">
-        <v>1.54</v>
+        <v>0</v>
       </c>
       <c r="D48" s="2">
         <v>2.58</v>
@@ -4584,13 +4595,13 @@
     </row>
     <row r="49" spans="1:4">
       <c r="A49" s="2" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="B49" s="2">
         <v>0.92</v>
       </c>
       <c r="C49" s="2">
-        <v>1.54</v>
+        <v>0</v>
       </c>
       <c r="D49" s="2">
         <v>2.46</v>
@@ -4601,24 +4612,23 @@
         <f>AVERAGE(B44:B49)</f>
         <v>0.76000000000000012</v>
       </c>
-      <c r="C50" s="3">
-        <f t="shared" ref="C50:D50" si="7">AVERAGE(C44:C49)</f>
-        <v>1.54</v>
+      <c r="C50" s="2">
+        <v>0</v>
       </c>
       <c r="D50" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" ref="C50:D50" si="7">AVERAGE(D44:D49)</f>
         <v>2.3000000000000003</v>
       </c>
     </row>
     <row r="51" spans="1:4">
       <c r="A51" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B51" s="2">
         <v>1.42</v>
       </c>
       <c r="C51" s="2">
-        <v>1.54</v>
+        <v>0</v>
       </c>
       <c r="D51" s="2">
         <v>2.96</v>
@@ -4626,13 +4636,13 @@
     </row>
     <row r="52" spans="1:4">
       <c r="A52" s="2" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B52" s="2">
         <v>1.0900000000000001</v>
       </c>
       <c r="C52" s="2">
-        <v>1.54</v>
+        <v>0</v>
       </c>
       <c r="D52" s="2">
         <v>2.63</v>
@@ -4640,13 +4650,13 @@
     </row>
     <row r="53" spans="1:4">
       <c r="A53" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B53" s="2">
         <v>0.45</v>
       </c>
       <c r="C53" s="2">
-        <v>1.54</v>
+        <v>0</v>
       </c>
       <c r="D53" s="2">
         <v>1.99</v>
@@ -4654,13 +4664,13 @@
     </row>
     <row r="54" spans="1:4">
       <c r="A54" s="2" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="B54" s="2">
         <v>0.19</v>
       </c>
       <c r="C54" s="2">
-        <v>1.54</v>
+        <v>0</v>
       </c>
       <c r="D54" s="2">
         <v>1.73</v>
@@ -4668,13 +4678,13 @@
     </row>
     <row r="55" spans="1:4">
       <c r="A55" s="2" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="B55" s="2">
         <v>1.35</v>
       </c>
       <c r="C55" s="2">
-        <v>1.54</v>
+        <v>0</v>
       </c>
       <c r="D55" s="2">
         <v>2.89</v>
@@ -4682,13 +4692,13 @@
     </row>
     <row r="56" spans="1:4">
       <c r="A56" s="2" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="B56" s="2">
         <v>1.1000000000000001</v>
       </c>
       <c r="C56" s="2">
-        <v>1.54</v>
+        <v>0</v>
       </c>
       <c r="D56" s="2">
         <v>2.64</v>
@@ -4699,24 +4709,23 @@
         <f>AVERAGE(B51:B56)</f>
         <v>0.93333333333333324</v>
       </c>
-      <c r="C57" s="3">
-        <f t="shared" ref="C57:D57" si="8">AVERAGE(C51:C56)</f>
-        <v>1.54</v>
+      <c r="C57" s="2">
+        <v>0</v>
       </c>
       <c r="D57" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" ref="C57:D57" si="8">AVERAGE(D51:D56)</f>
         <v>2.4733333333333336</v>
       </c>
     </row>
     <row r="58" spans="1:4">
       <c r="A58" s="2" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B58" s="2">
         <v>1.62</v>
       </c>
       <c r="C58" s="2">
-        <v>1.54</v>
+        <v>0</v>
       </c>
       <c r="D58" s="2">
         <v>3.16</v>
@@ -4724,13 +4733,13 @@
     </row>
     <row r="59" spans="1:4">
       <c r="A59" s="2" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B59" s="2">
         <v>1.26</v>
       </c>
       <c r="C59" s="2">
-        <v>1.54</v>
+        <v>0</v>
       </c>
       <c r="D59" s="2">
         <v>2.8</v>
@@ -4738,13 +4747,13 @@
     </row>
     <row r="60" spans="1:4">
       <c r="A60" s="2" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B60" s="2">
         <v>0.43</v>
       </c>
       <c r="C60" s="2">
-        <v>1.54</v>
+        <v>0</v>
       </c>
       <c r="D60" s="2">
         <v>1.97</v>
@@ -4752,13 +4761,13 @@
     </row>
     <row r="61" spans="1:4">
       <c r="A61" s="2" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="B61" s="2">
         <v>0.26</v>
       </c>
       <c r="C61" s="2">
-        <v>1.54</v>
+        <v>0</v>
       </c>
       <c r="D61" s="2">
         <v>1.8</v>
@@ -4766,13 +4775,13 @@
     </row>
     <row r="62" spans="1:4">
       <c r="A62" s="2" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B62" s="2">
         <v>1.53</v>
       </c>
       <c r="C62" s="2">
-        <v>1.54</v>
+        <v>0</v>
       </c>
       <c r="D62" s="2">
         <v>3.07</v>
@@ -4780,13 +4789,13 @@
     </row>
     <row r="63" spans="1:4">
       <c r="A63" s="2" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="B63" s="2">
         <v>1.25</v>
       </c>
       <c r="C63" s="2">
-        <v>1.54</v>
+        <v>0</v>
       </c>
       <c r="D63" s="2">
         <v>2.79</v>
@@ -4797,24 +4806,23 @@
         <f>AVERAGE(B58:B63)</f>
         <v>1.0583333333333333</v>
       </c>
-      <c r="C64" s="3">
-        <f t="shared" ref="C64:D64" si="9">AVERAGE(C58:C63)</f>
-        <v>1.54</v>
+      <c r="C64" s="2">
+        <v>0</v>
       </c>
       <c r="D64" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" ref="C64:D64" si="9">AVERAGE(D58:D63)</f>
         <v>2.5983333333333332</v>
       </c>
     </row>
     <row r="65" spans="1:4">
       <c r="A65" s="2" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B65" s="2">
         <v>1.64</v>
       </c>
       <c r="C65" s="2">
-        <v>1.54</v>
+        <v>0</v>
       </c>
       <c r="D65" s="2">
         <v>3.18</v>
@@ -4822,13 +4830,13 @@
     </row>
     <row r="66" spans="1:4">
       <c r="A66" s="2" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B66" s="2">
         <v>1.1100000000000001</v>
       </c>
       <c r="C66" s="2">
-        <v>1.54</v>
+        <v>0</v>
       </c>
       <c r="D66" s="2">
         <v>2.65</v>
@@ -4836,13 +4844,13 @@
     </row>
     <row r="67" spans="1:4">
       <c r="A67" s="2" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B67" s="2">
         <v>0.44</v>
       </c>
       <c r="C67" s="2">
-        <v>1.54</v>
+        <v>0</v>
       </c>
       <c r="D67" s="2">
         <v>1.98</v>
@@ -4850,13 +4858,13 @@
     </row>
     <row r="68" spans="1:4">
       <c r="A68" s="2" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="B68" s="2">
         <v>0.27</v>
       </c>
       <c r="C68" s="2">
-        <v>1.54</v>
+        <v>0</v>
       </c>
       <c r="D68" s="2">
         <v>1.81</v>
@@ -4864,13 +4872,13 @@
     </row>
     <row r="69" spans="1:4">
       <c r="A69" s="2" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="B69" s="2">
         <v>1.44</v>
       </c>
       <c r="C69" s="2">
-        <v>1.54</v>
+        <v>0</v>
       </c>
       <c r="D69" s="2">
         <v>2.98</v>
@@ -4878,13 +4886,13 @@
     </row>
     <row r="70" spans="1:4">
       <c r="A70" s="2" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="B70" s="2">
         <v>1.2</v>
       </c>
       <c r="C70" s="2">
-        <v>1.54</v>
+        <v>0</v>
       </c>
       <c r="D70" s="2">
         <v>2.74</v>
@@ -4895,9 +4903,8 @@
         <f>AVERAGE(B65:B70)</f>
         <v>1.0166666666666668</v>
       </c>
-      <c r="C71" s="3">
-        <f>AVERAGE(C65:C70)</f>
-        <v>1.54</v>
+      <c r="C71" s="2">
+        <v>0</v>
       </c>
       <c r="D71" s="3">
         <f>AVERAGE(D65:D70)</f>
@@ -4906,13 +4913,13 @@
     </row>
     <row r="72" spans="1:4">
       <c r="A72" s="2" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B72" s="2">
         <v>1.62</v>
       </c>
       <c r="C72" s="2">
-        <v>1.54</v>
+        <v>0</v>
       </c>
       <c r="D72" s="2">
         <v>3.16</v>
@@ -4920,13 +4927,13 @@
     </row>
     <row r="73" spans="1:4">
       <c r="A73" s="2" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B73" s="2">
         <v>0.96</v>
       </c>
       <c r="C73" s="2">
-        <v>1.54</v>
+        <v>0</v>
       </c>
       <c r="D73" s="2">
         <v>2.5</v>
@@ -4934,13 +4941,13 @@
     </row>
     <row r="74" spans="1:4">
       <c r="A74" s="2" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B74" s="2">
         <v>0.38</v>
       </c>
       <c r="C74" s="2">
-        <v>1.54</v>
+        <v>0</v>
       </c>
       <c r="D74" s="2">
         <v>1.92</v>
@@ -4948,13 +4955,13 @@
     </row>
     <row r="75" spans="1:4">
       <c r="A75" s="2" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B75" s="2">
         <v>0.37</v>
       </c>
       <c r="C75" s="2">
-        <v>1.54</v>
+        <v>0</v>
       </c>
       <c r="D75" s="2">
         <v>1.91</v>
@@ -4962,13 +4969,13 @@
     </row>
     <row r="76" spans="1:4">
       <c r="A76" s="2" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="B76" s="2">
         <v>1.41</v>
       </c>
       <c r="C76" s="2">
-        <v>1.54</v>
+        <v>0</v>
       </c>
       <c r="D76" s="2">
         <v>2.95</v>
@@ -4976,13 +4983,13 @@
     </row>
     <row r="77" spans="1:4">
       <c r="A77" s="2" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="B77" s="2">
         <v>1.17</v>
       </c>
       <c r="C77" s="2">
-        <v>1.54</v>
+        <v>0</v>
       </c>
       <c r="D77" s="2">
         <v>2.71</v>
@@ -4993,9 +5000,8 @@
         <f>AVERAGE(B72:B77)</f>
         <v>0.98499999999999999</v>
       </c>
-      <c r="C78" s="3">
-        <f>AVERAGE(C72:C77)</f>
-        <v>1.54</v>
+      <c r="C78" s="2">
+        <v>0</v>
       </c>
       <c r="D78" s="3">
         <f>AVERAGE(D72:D77)</f>
@@ -5004,13 +5010,13 @@
     </row>
     <row r="79" spans="1:4">
       <c r="A79" s="2" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B79" s="2">
         <v>1.58</v>
       </c>
       <c r="C79" s="2">
-        <v>1.54</v>
+        <v>0</v>
       </c>
       <c r="D79" s="2">
         <v>3.12</v>
@@ -5018,13 +5024,13 @@
     </row>
     <row r="80" spans="1:4">
       <c r="A80" s="2" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B80" s="2">
         <v>0.92</v>
       </c>
       <c r="C80" s="2">
-        <v>1.54</v>
+        <v>0</v>
       </c>
       <c r="D80" s="2">
         <v>2.46</v>
@@ -5032,13 +5038,13 @@
     </row>
     <row r="81" spans="1:4">
       <c r="A81" s="2" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B81" s="2">
         <v>0.34</v>
       </c>
       <c r="C81" s="2">
-        <v>1.54</v>
+        <v>0</v>
       </c>
       <c r="D81" s="2">
         <v>1.88</v>
@@ -5046,13 +5052,13 @@
     </row>
     <row r="82" spans="1:4">
       <c r="A82" s="2" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="B82" s="2">
         <v>0.41</v>
       </c>
       <c r="C82" s="2">
-        <v>1.54</v>
+        <v>0</v>
       </c>
       <c r="D82" s="2">
         <v>1.95</v>
@@ -5060,13 +5066,13 @@
     </row>
     <row r="83" spans="1:4">
       <c r="A83" s="2" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="B83" s="2">
         <v>1.1599999999999999</v>
       </c>
       <c r="C83" s="2">
-        <v>1.54</v>
+        <v>0</v>
       </c>
       <c r="D83" s="2">
         <v>2.7</v>
@@ -5074,13 +5080,13 @@
     </row>
     <row r="84" spans="1:4">
       <c r="A84" s="2" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="B84" s="2">
         <v>1.2</v>
       </c>
       <c r="C84" s="2">
-        <v>1.54</v>
+        <v>0</v>
       </c>
       <c r="D84" s="2">
         <v>2.74</v>
@@ -5091,9 +5097,8 @@
         <f>AVERAGE(B79:B84)</f>
         <v>0.93500000000000005</v>
       </c>
-      <c r="C85" s="3">
-        <f>AVERAGE(C79:C84)</f>
-        <v>1.54</v>
+      <c r="C85" s="2">
+        <v>0</v>
       </c>
       <c r="D85" s="3">
         <f>AVERAGE(D79:D84)</f>
@@ -5102,13 +5107,13 @@
     </row>
     <row r="86" spans="1:4">
       <c r="A86" s="2" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B86" s="2">
         <v>1.54</v>
       </c>
       <c r="C86" s="2">
-        <v>1.54</v>
+        <v>0</v>
       </c>
       <c r="D86" s="2">
         <v>3.08</v>
@@ -5116,13 +5121,13 @@
     </row>
     <row r="87" spans="1:4">
       <c r="A87" s="2" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B87" s="2">
         <v>0.88</v>
       </c>
       <c r="C87" s="2">
-        <v>1.54</v>
+        <v>0</v>
       </c>
       <c r="D87" s="2">
         <v>2.42</v>
@@ -5130,13 +5135,13 @@
     </row>
     <row r="88" spans="1:4">
       <c r="A88" s="2" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B88" s="2">
         <v>0.34</v>
       </c>
       <c r="C88" s="2">
-        <v>1.54</v>
+        <v>0</v>
       </c>
       <c r="D88" s="2">
         <v>1.88</v>
@@ -5144,13 +5149,13 @@
     </row>
     <row r="89" spans="1:4">
       <c r="A89" s="2" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="B89" s="2">
         <v>0.42</v>
       </c>
       <c r="C89" s="2">
-        <v>1.54</v>
+        <v>0</v>
       </c>
       <c r="D89" s="2">
         <v>1.96</v>
@@ -5158,13 +5163,13 @@
     </row>
     <row r="90" spans="1:4">
       <c r="A90" s="2" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="B90" s="2">
         <v>1.1100000000000001</v>
       </c>
       <c r="C90" s="2">
-        <v>1.54</v>
+        <v>0</v>
       </c>
       <c r="D90" s="2">
         <v>2.65</v>
@@ -5172,13 +5177,13 @@
     </row>
     <row r="91" spans="1:4">
       <c r="A91" s="2" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="B91" s="2">
         <v>1.22</v>
       </c>
       <c r="C91" s="2">
-        <v>1.54</v>
+        <v>0</v>
       </c>
       <c r="D91" s="2">
         <v>2.76</v>
@@ -5189,24 +5194,23 @@
         <f>AVERAGE(B86:B91)</f>
         <v>0.91833333333333333</v>
       </c>
-      <c r="C92" s="3">
-        <f t="shared" ref="C92:D92" si="10">AVERAGE(C86:C91)</f>
-        <v>1.54</v>
+      <c r="C92" s="2">
+        <v>0</v>
       </c>
       <c r="D92" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" ref="C92:D92" si="10">AVERAGE(D86:D91)</f>
         <v>2.4583333333333335</v>
       </c>
     </row>
     <row r="93" spans="1:4">
       <c r="A93" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B93" s="2">
         <v>1.51</v>
       </c>
       <c r="C93" s="2">
-        <v>1.54</v>
+        <v>0</v>
       </c>
       <c r="D93" s="2">
         <v>3.05</v>
@@ -5214,13 +5218,13 @@
     </row>
     <row r="94" spans="1:4">
       <c r="A94" s="2" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B94" s="2">
         <v>0.81</v>
       </c>
       <c r="C94" s="2">
-        <v>1.54</v>
+        <v>0</v>
       </c>
       <c r="D94" s="2">
         <v>2.35</v>
@@ -5228,13 +5232,13 @@
     </row>
     <row r="95" spans="1:4">
       <c r="A95" s="2" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B95" s="2">
         <v>0.3</v>
       </c>
       <c r="C95" s="2">
-        <v>1.54</v>
+        <v>0</v>
       </c>
       <c r="D95" s="2">
         <v>1.84</v>
@@ -5242,13 +5246,13 @@
     </row>
     <row r="96" spans="1:4">
       <c r="A96" s="2" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B96" s="2">
         <v>0.41</v>
       </c>
       <c r="C96" s="2">
-        <v>1.54</v>
+        <v>0</v>
       </c>
       <c r="D96" s="2">
         <v>1.95</v>
@@ -5256,13 +5260,13 @@
     </row>
     <row r="97" spans="1:4">
       <c r="A97" s="2" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="B97" s="2">
         <v>1.06</v>
       </c>
       <c r="C97" s="2">
-        <v>1.54</v>
+        <v>0</v>
       </c>
       <c r="D97" s="2">
         <v>2.6</v>
@@ -5270,13 +5274,13 @@
     </row>
     <row r="98" spans="1:4">
       <c r="A98" s="2" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="B98" s="2">
         <v>1.35</v>
       </c>
       <c r="C98" s="2">
-        <v>1.54</v>
+        <v>0</v>
       </c>
       <c r="D98" s="2">
         <v>2.89</v>
@@ -5287,24 +5291,23 @@
         <f>AVERAGE(B93:B98)</f>
         <v>0.90666666666666662</v>
       </c>
-      <c r="C99" s="3">
-        <f t="shared" ref="C99:D99" si="11">AVERAGE(C93:C98)</f>
-        <v>1.54</v>
+      <c r="C99" s="2">
+        <v>0</v>
       </c>
       <c r="D99" s="3">
-        <f t="shared" si="11"/>
+        <f t="shared" ref="C99:D99" si="11">AVERAGE(D93:D98)</f>
         <v>2.4466666666666668</v>
       </c>
     </row>
     <row r="100" spans="1:4">
       <c r="A100" s="2" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B100" s="2">
         <v>1.47</v>
       </c>
       <c r="C100" s="2">
-        <v>1.54</v>
+        <v>0</v>
       </c>
       <c r="D100" s="2">
         <v>3.01</v>
@@ -5312,13 +5315,13 @@
     </row>
     <row r="101" spans="1:4">
       <c r="A101" s="2" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B101" s="2">
         <v>0.93</v>
       </c>
       <c r="C101" s="2">
-        <v>1.54</v>
+        <v>0</v>
       </c>
       <c r="D101" s="2">
         <v>2.4700000000000002</v>
@@ -5326,13 +5329,13 @@
     </row>
     <row r="102" spans="1:4">
       <c r="A102" s="2" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B102" s="2">
         <v>0.51</v>
       </c>
       <c r="C102" s="2">
-        <v>1.54</v>
+        <v>0</v>
       </c>
       <c r="D102" s="2">
         <v>2.0499999999999998</v>
@@ -5340,13 +5343,13 @@
     </row>
     <row r="103" spans="1:4">
       <c r="A103" s="2" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="B103" s="2">
         <v>0.43</v>
       </c>
       <c r="C103" s="2">
-        <v>1.54</v>
+        <v>0</v>
       </c>
       <c r="D103" s="2">
         <v>1.97</v>
@@ -5354,13 +5357,13 @@
     </row>
     <row r="104" spans="1:4">
       <c r="A104" s="2" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="B104" s="2">
         <v>1.04</v>
       </c>
       <c r="C104" s="2">
-        <v>1.54</v>
+        <v>0</v>
       </c>
       <c r="D104" s="2">
         <v>2.58</v>
@@ -5368,13 +5371,13 @@
     </row>
     <row r="105" spans="1:4">
       <c r="A105" s="2" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="B105" s="2">
         <v>1.41</v>
       </c>
       <c r="C105" s="2">
-        <v>1.54</v>
+        <v>0</v>
       </c>
       <c r="D105" s="2">
         <v>2.95</v>
@@ -5385,24 +5388,23 @@
         <f>AVERAGE(B100:B105)</f>
         <v>0.96500000000000019</v>
       </c>
-      <c r="C106" s="3">
-        <f t="shared" ref="C106:D106" si="12">AVERAGE(C100:C105)</f>
-        <v>1.54</v>
+      <c r="C106" s="2">
+        <v>0</v>
       </c>
       <c r="D106" s="3">
-        <f t="shared" si="12"/>
+        <f t="shared" ref="C106:D106" si="12">AVERAGE(D100:D105)</f>
         <v>2.5050000000000003</v>
       </c>
     </row>
     <row r="107" spans="1:4">
       <c r="A107" s="2" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B107" s="2">
         <v>1.38</v>
       </c>
       <c r="C107" s="2">
-        <v>1.54</v>
+        <v>0</v>
       </c>
       <c r="D107" s="2">
         <v>2.92</v>
@@ -5410,13 +5412,13 @@
     </row>
     <row r="108" spans="1:4">
       <c r="A108" s="2" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B108" s="2">
         <v>1.22</v>
       </c>
       <c r="C108" s="2">
-        <v>1.54</v>
+        <v>0</v>
       </c>
       <c r="D108" s="2">
         <v>2.76</v>
@@ -5424,13 +5426,13 @@
     </row>
     <row r="109" spans="1:4">
       <c r="A109" s="2" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B109" s="2">
         <v>0.47</v>
       </c>
       <c r="C109" s="2">
-        <v>1.54</v>
+        <v>0</v>
       </c>
       <c r="D109" s="2">
         <v>2.0099999999999998</v>
@@ -5438,13 +5440,13 @@
     </row>
     <row r="110" spans="1:4">
       <c r="A110" s="2" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="B110" s="2">
         <v>0.5</v>
       </c>
       <c r="C110" s="2">
-        <v>1.54</v>
+        <v>0</v>
       </c>
       <c r="D110" s="2">
         <v>2.04</v>
@@ -5452,13 +5454,13 @@
     </row>
     <row r="111" spans="1:4">
       <c r="A111" s="2" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="B111" s="2">
         <v>1.04</v>
       </c>
       <c r="C111" s="2">
-        <v>1.54</v>
+        <v>0</v>
       </c>
       <c r="D111" s="2">
         <v>2.58</v>
@@ -5466,13 +5468,13 @@
     </row>
     <row r="112" spans="1:4">
       <c r="A112" s="2" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="B112" s="2">
         <v>1.48</v>
       </c>
       <c r="C112" s="2">
-        <v>1.54</v>
+        <v>0</v>
       </c>
       <c r="D112" s="2">
         <v>3.02</v>
@@ -5483,24 +5485,23 @@
         <f>AVERAGE(B107:B112)</f>
         <v>1.0149999999999999</v>
       </c>
-      <c r="C113" s="3">
-        <f t="shared" ref="C113:D113" si="13">AVERAGE(C107:C112)</f>
-        <v>1.54</v>
+      <c r="C113" s="2">
+        <v>0</v>
       </c>
       <c r="D113" s="3">
-        <f t="shared" si="13"/>
+        <f t="shared" ref="C113:D113" si="13">AVERAGE(D107:D112)</f>
         <v>2.5550000000000002</v>
       </c>
     </row>
     <row r="114" spans="1:4">
       <c r="A114" s="2" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B114" s="2">
         <v>1.4</v>
       </c>
       <c r="C114" s="2">
-        <v>1.54</v>
+        <v>0</v>
       </c>
       <c r="D114" s="2">
         <v>2.94</v>
@@ -5508,13 +5509,13 @@
     </row>
     <row r="115" spans="1:4">
       <c r="A115" s="2" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B115" s="2">
         <v>1.38</v>
       </c>
       <c r="C115" s="2">
-        <v>1.54</v>
+        <v>0</v>
       </c>
       <c r="D115" s="2">
         <v>2.92</v>
@@ -5522,13 +5523,13 @@
     </row>
     <row r="116" spans="1:4">
       <c r="A116" s="2" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B116" s="2">
         <v>0.52</v>
       </c>
       <c r="C116" s="2">
-        <v>1.54</v>
+        <v>0</v>
       </c>
       <c r="D116" s="2">
         <v>2.06</v>
@@ -5536,13 +5537,13 @@
     </row>
     <row r="117" spans="1:4">
       <c r="A117" s="2" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B117" s="2">
         <v>0.52</v>
       </c>
       <c r="C117" s="2">
-        <v>1.54</v>
+        <v>0</v>
       </c>
       <c r="D117" s="2">
         <v>2.06</v>
@@ -5550,13 +5551,13 @@
     </row>
     <row r="118" spans="1:4">
       <c r="A118" s="2" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="B118" s="2">
         <v>1.05</v>
       </c>
       <c r="C118" s="2">
-        <v>1.54</v>
+        <v>0</v>
       </c>
       <c r="D118" s="2">
         <v>2.59</v>
@@ -5564,13 +5565,13 @@
     </row>
     <row r="119" spans="1:4">
       <c r="A119" s="2" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="B119" s="2">
         <v>1.53</v>
       </c>
       <c r="C119" s="2">
-        <v>1.54</v>
+        <v>0</v>
       </c>
       <c r="D119" s="2">
         <v>3.07</v>
@@ -5581,24 +5582,23 @@
         <f>AVERAGE(B114:B119)</f>
         <v>1.0666666666666667</v>
       </c>
-      <c r="C120" s="3">
-        <f t="shared" ref="C120:D120" si="14">AVERAGE(C114:C119)</f>
-        <v>1.54</v>
+      <c r="C120" s="2">
+        <v>0</v>
       </c>
       <c r="D120" s="3">
-        <f t="shared" si="14"/>
+        <f t="shared" ref="C120:D120" si="14">AVERAGE(D114:D119)</f>
         <v>2.6066666666666669</v>
       </c>
     </row>
     <row r="121" spans="1:4">
       <c r="A121" s="2" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B121" s="2">
         <v>1.48</v>
       </c>
       <c r="C121" s="2">
-        <v>2.4</v>
+        <v>0</v>
       </c>
       <c r="D121" s="2">
         <v>3.88</v>
@@ -5606,13 +5606,13 @@
     </row>
     <row r="122" spans="1:4">
       <c r="A122" s="2" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B122" s="2">
         <v>1.64</v>
       </c>
       <c r="C122" s="2">
-        <v>2.4</v>
+        <v>0</v>
       </c>
       <c r="D122" s="2">
         <v>4.04</v>
@@ -5620,13 +5620,13 @@
     </row>
     <row r="123" spans="1:4">
       <c r="A123" s="2" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B123" s="2">
         <v>0.53</v>
       </c>
       <c r="C123" s="2">
-        <v>2.4</v>
+        <v>0</v>
       </c>
       <c r="D123" s="2">
         <v>2.93</v>
@@ -5634,13 +5634,13 @@
     </row>
     <row r="124" spans="1:4">
       <c r="A124" s="2" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="B124" s="2">
         <v>0.6</v>
       </c>
       <c r="C124" s="2">
-        <v>2.4</v>
+        <v>0</v>
       </c>
       <c r="D124" s="2">
         <v>3</v>
@@ -5648,13 +5648,13 @@
     </row>
     <row r="125" spans="1:4">
       <c r="A125" s="2" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="B125" s="2">
         <v>1.0900000000000001</v>
       </c>
       <c r="C125" s="2">
-        <v>2.4</v>
+        <v>0</v>
       </c>
       <c r="D125" s="2">
         <v>3.49</v>
@@ -5662,13 +5662,13 @@
     </row>
     <row r="126" spans="1:4">
       <c r="A126" s="2" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="B126" s="2">
         <v>1.61</v>
       </c>
       <c r="C126" s="2">
-        <v>2.4</v>
+        <v>0</v>
       </c>
       <c r="D126" s="2">
         <v>4.01</v>
@@ -5679,24 +5679,23 @@
         <f>AVERAGE(B121:B126)</f>
         <v>1.1583333333333334</v>
       </c>
-      <c r="C127" s="3">
-        <f t="shared" ref="C127:D127" si="15">AVERAGE(C121:C126)</f>
-        <v>2.4</v>
+      <c r="C127" s="2">
+        <v>0</v>
       </c>
       <c r="D127" s="3">
-        <f t="shared" si="15"/>
+        <f t="shared" ref="C127:D127" si="15">AVERAGE(D121:D126)</f>
         <v>3.5583333333333336</v>
       </c>
     </row>
     <row r="128" spans="1:4">
       <c r="A128" s="2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B128" s="2">
         <v>1.4</v>
       </c>
       <c r="C128" s="2">
-        <v>2.4</v>
+        <v>0</v>
       </c>
       <c r="D128" s="2">
         <v>3.8</v>
@@ -5704,13 +5703,13 @@
     </row>
     <row r="129" spans="1:4">
       <c r="A129" s="2" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B129" s="2">
         <v>1.67</v>
       </c>
       <c r="C129" s="2">
-        <v>2.4</v>
+        <v>0</v>
       </c>
       <c r="D129" s="2">
         <v>4.07</v>
@@ -5718,13 +5717,13 @@
     </row>
     <row r="130" spans="1:4">
       <c r="A130" s="2" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B130" s="2">
         <v>0.52</v>
       </c>
       <c r="C130" s="2">
-        <v>2.4</v>
+        <v>0</v>
       </c>
       <c r="D130" s="2">
         <v>2.92</v>
@@ -5732,13 +5731,13 @@
     </row>
     <row r="131" spans="1:4">
       <c r="A131" s="2" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B131" s="2">
         <v>0.57999999999999996</v>
       </c>
       <c r="C131" s="2">
-        <v>2.4</v>
+        <v>0</v>
       </c>
       <c r="D131" s="2">
         <v>2.98</v>
@@ -5746,13 +5745,13 @@
     </row>
     <row r="132" spans="1:4">
       <c r="A132" s="2" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="B132" s="2">
         <v>0.87</v>
       </c>
       <c r="C132" s="2">
-        <v>2.4</v>
+        <v>0</v>
       </c>
       <c r="D132" s="2">
         <v>3.27</v>
@@ -5760,13 +5759,13 @@
     </row>
     <row r="133" spans="1:4">
       <c r="A133" s="2" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="B133" s="2">
         <v>1.6</v>
       </c>
       <c r="C133" s="2">
-        <v>2.4</v>
+        <v>0</v>
       </c>
       <c r="D133" s="2">
         <v>4</v>
@@ -5777,24 +5776,23 @@
         <f>AVERAGE(B128:B133)</f>
         <v>1.1066666666666667</v>
       </c>
-      <c r="C134" s="3">
-        <f t="shared" ref="C134:D134" si="16">AVERAGE(C128:C133)</f>
-        <v>2.4</v>
+      <c r="C134" s="2">
+        <v>0</v>
       </c>
       <c r="D134" s="3">
-        <f t="shared" si="16"/>
+        <f t="shared" ref="C134:D134" si="16">AVERAGE(D128:D133)</f>
         <v>3.5066666666666664</v>
       </c>
     </row>
     <row r="135" spans="1:4">
       <c r="A135" s="2" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B135" s="2">
         <v>1.33</v>
       </c>
       <c r="C135" s="2">
-        <v>2.4</v>
+        <v>0</v>
       </c>
       <c r="D135" s="2">
         <v>3.73</v>
@@ -5802,13 +5800,13 @@
     </row>
     <row r="136" spans="1:4">
       <c r="A136" s="2" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B136" s="2">
         <v>1.57</v>
       </c>
       <c r="C136" s="2">
-        <v>2.4</v>
+        <v>0</v>
       </c>
       <c r="D136" s="2">
         <v>3.97</v>
@@ -5816,13 +5814,13 @@
     </row>
     <row r="137" spans="1:4">
       <c r="A137" s="2" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B137" s="2">
         <v>0.51</v>
       </c>
       <c r="C137" s="2">
-        <v>2.4</v>
+        <v>0</v>
       </c>
       <c r="D137" s="2">
         <v>2.91</v>
@@ -5830,13 +5828,13 @@
     </row>
     <row r="138" spans="1:4">
       <c r="A138" s="2" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="B138" s="2">
         <v>0.53</v>
       </c>
       <c r="C138" s="2">
-        <v>2.4</v>
+        <v>0</v>
       </c>
       <c r="D138" s="2">
         <v>2.93</v>
@@ -5844,13 +5842,13 @@
     </row>
     <row r="139" spans="1:4">
       <c r="A139" s="2" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="B139" s="2">
         <v>0.53</v>
       </c>
       <c r="C139" s="2">
-        <v>2.4</v>
+        <v>0</v>
       </c>
       <c r="D139" s="2">
         <v>2.93</v>
@@ -5858,13 +5856,13 @@
     </row>
     <row r="140" spans="1:4">
       <c r="A140" s="2" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="B140" s="2">
         <v>1.54</v>
       </c>
       <c r="C140" s="2">
-        <v>2.4</v>
+        <v>0</v>
       </c>
       <c r="D140" s="2">
         <v>3.94</v>
@@ -5875,24 +5873,23 @@
         <f>AVERAGE(B135:B140)</f>
         <v>1.0016666666666667</v>
       </c>
-      <c r="C141" s="3">
-        <f t="shared" ref="C141:D141" si="17">AVERAGE(C135:C140)</f>
-        <v>2.4</v>
+      <c r="C141" s="2">
+        <v>0</v>
       </c>
       <c r="D141" s="3">
-        <f t="shared" si="17"/>
+        <f t="shared" ref="C141:D141" si="17">AVERAGE(D135:D140)</f>
         <v>3.4016666666666668</v>
       </c>
     </row>
     <row r="142" spans="1:4">
       <c r="A142" s="2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B142" s="2">
         <v>1.25</v>
       </c>
       <c r="C142" s="2">
-        <v>2.4</v>
+        <v>0</v>
       </c>
       <c r="D142" s="2">
         <v>3.65</v>
@@ -5900,13 +5897,13 @@
     </row>
     <row r="143" spans="1:4">
       <c r="A143" s="2" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B143" s="2">
         <v>1.35</v>
       </c>
       <c r="C143" s="2">
-        <v>2.4</v>
+        <v>0</v>
       </c>
       <c r="D143" s="2">
         <v>3.75</v>
@@ -5914,13 +5911,13 @@
     </row>
     <row r="144" spans="1:4">
       <c r="A144" s="2" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B144" s="2">
         <v>0.5</v>
       </c>
       <c r="C144" s="2">
-        <v>2.4</v>
+        <v>0</v>
       </c>
       <c r="D144" s="2">
         <v>2.9</v>
@@ -5928,13 +5925,13 @@
     </row>
     <row r="145" spans="1:4">
       <c r="A145" s="2" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B145" s="2">
         <v>0.5</v>
       </c>
       <c r="C145" s="2">
-        <v>2.4</v>
+        <v>0</v>
       </c>
       <c r="D145" s="2">
         <v>2.9</v>
@@ -5942,13 +5939,13 @@
     </row>
     <row r="146" spans="1:4">
       <c r="A146" s="2" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="B146" s="2">
         <v>0.53</v>
       </c>
       <c r="C146" s="2">
-        <v>2.4</v>
+        <v>0</v>
       </c>
       <c r="D146" s="2">
         <v>2.93</v>
@@ -5956,13 +5953,13 @@
     </row>
     <row r="147" spans="1:4">
       <c r="A147" s="2" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="B147" s="2">
         <v>1.45</v>
       </c>
       <c r="C147" s="2">
-        <v>2.4</v>
+        <v>0</v>
       </c>
       <c r="D147" s="2">
         <v>3.85</v>
@@ -5973,24 +5970,23 @@
         <f>AVERAGE(B142:B147)</f>
         <v>0.93</v>
       </c>
-      <c r="C148" s="3">
-        <f t="shared" ref="C148:D148" si="18">AVERAGE(C142:C147)</f>
-        <v>2.4</v>
+      <c r="C148" s="2">
+        <v>0</v>
       </c>
       <c r="D148" s="3">
-        <f t="shared" si="18"/>
+        <f t="shared" ref="C148:D148" si="18">AVERAGE(D142:D147)</f>
         <v>3.3300000000000005</v>
       </c>
     </row>
     <row r="149" spans="1:4">
       <c r="A149" s="2" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B149" s="2">
         <v>1.26</v>
       </c>
       <c r="C149" s="2">
-        <v>1.54</v>
+        <v>0</v>
       </c>
       <c r="D149" s="2">
         <v>2.8</v>
@@ -5998,13 +5994,13 @@
     </row>
     <row r="150" spans="1:4">
       <c r="A150" s="2" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B150" s="2">
         <v>0.49</v>
       </c>
       <c r="C150" s="2">
-        <v>1.54</v>
+        <v>0</v>
       </c>
       <c r="D150" s="2">
         <v>2.0299999999999998</v>
@@ -6012,13 +6008,13 @@
     </row>
     <row r="151" spans="1:4">
       <c r="A151" s="2" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="B151" s="2">
         <v>0.52</v>
       </c>
       <c r="C151" s="2">
-        <v>1.54</v>
+        <v>0</v>
       </c>
       <c r="D151" s="2">
         <v>2.06</v>
@@ -6026,13 +6022,13 @@
     </row>
     <row r="152" spans="1:4">
       <c r="A152" s="2" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="B152" s="2">
         <v>0.46</v>
       </c>
       <c r="C152" s="2">
-        <v>1.54</v>
+        <v>0</v>
       </c>
       <c r="D152" s="2">
         <v>2</v>
@@ -6040,13 +6036,13 @@
     </row>
     <row r="153" spans="1:4">
       <c r="A153" s="2" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="B153" s="2">
         <v>1.37</v>
       </c>
       <c r="C153" s="2">
-        <v>1.54</v>
+        <v>0</v>
       </c>
       <c r="D153" s="2">
         <v>2.91</v>
@@ -6057,24 +6053,23 @@
         <f>AVERAGE(B149:B153)</f>
         <v>0.82</v>
       </c>
-      <c r="C154" s="3">
-        <f t="shared" ref="C154:D154" si="19">AVERAGE(C149:C153)</f>
-        <v>1.54</v>
+      <c r="C154" s="2">
+        <v>0</v>
       </c>
       <c r="D154" s="3">
-        <f t="shared" si="19"/>
+        <f t="shared" ref="C154:D154" si="19">AVERAGE(D149:D153)</f>
         <v>2.3600000000000003</v>
       </c>
     </row>
     <row r="155" spans="1:4">
       <c r="A155" s="2" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B155" s="2">
         <v>1.1399999999999999</v>
       </c>
       <c r="C155" s="2">
-        <v>1.54</v>
+        <v>0</v>
       </c>
       <c r="D155" s="2">
         <v>2.68</v>
@@ -6082,13 +6077,13 @@
     </row>
     <row r="156" spans="1:4">
       <c r="A156" s="2" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B156" s="2">
         <v>1.25</v>
       </c>
       <c r="C156" s="2">
-        <v>1.54</v>
+        <v>0</v>
       </c>
       <c r="D156" s="2">
         <v>2.79</v>
@@ -6096,13 +6091,13 @@
     </row>
     <row r="157" spans="1:4">
       <c r="A157" s="2" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B157" s="2">
         <v>0.45</v>
       </c>
       <c r="C157" s="2">
-        <v>1.54</v>
+        <v>0</v>
       </c>
       <c r="D157" s="2">
         <v>1.99</v>
@@ -6110,13 +6105,13 @@
     </row>
     <row r="158" spans="1:4">
       <c r="A158" s="2" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="B158" s="2">
         <v>0.47</v>
       </c>
       <c r="C158" s="2">
-        <v>1.54</v>
+        <v>0</v>
       </c>
       <c r="D158" s="2">
         <v>2.0099999999999998</v>
@@ -6124,13 +6119,13 @@
     </row>
     <row r="159" spans="1:4">
       <c r="A159" s="2" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="B159" s="2">
         <v>0.31</v>
       </c>
       <c r="C159" s="2">
-        <v>1.54</v>
+        <v>0</v>
       </c>
       <c r="D159" s="2">
         <v>1.85</v>
@@ -6138,13 +6133,13 @@
     </row>
     <row r="160" spans="1:4">
       <c r="A160" s="2" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="B160" s="2">
         <v>1.3</v>
       </c>
       <c r="C160" s="2">
-        <v>1.54</v>
+        <v>0</v>
       </c>
       <c r="D160" s="2">
         <v>2.84</v>
@@ -6155,24 +6150,23 @@
         <f>AVERAGE(B155:B160)</f>
         <v>0.82</v>
       </c>
-      <c r="C161" s="3">
-        <f t="shared" ref="C161:D161" si="20">AVERAGE(C155:C160)</f>
-        <v>1.54</v>
+      <c r="C161" s="2">
+        <v>0</v>
       </c>
       <c r="D161" s="3">
-        <f t="shared" si="20"/>
+        <f t="shared" ref="C161:D161" si="20">AVERAGE(D155:D160)</f>
         <v>2.36</v>
       </c>
     </row>
     <row r="162" spans="1:4">
       <c r="A162" s="2" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B162" s="2">
         <v>1</v>
       </c>
       <c r="C162" s="2">
-        <v>1.54</v>
+        <v>0</v>
       </c>
       <c r="D162" s="2">
         <v>2.54</v>
@@ -6180,13 +6174,13 @@
     </row>
     <row r="163" spans="1:4">
       <c r="A163" s="2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B163" s="2">
         <v>1.17</v>
       </c>
       <c r="C163" s="2">
-        <v>1.54</v>
+        <v>0</v>
       </c>
       <c r="D163" s="2">
         <v>2.71</v>
@@ -6194,13 +6188,13 @@
     </row>
     <row r="164" spans="1:4">
       <c r="A164" s="2" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B164" s="2">
         <v>0.38</v>
       </c>
       <c r="C164" s="2">
-        <v>1.54</v>
+        <v>0</v>
       </c>
       <c r="D164" s="2">
         <v>1.92</v>
@@ -6208,13 +6202,13 @@
     </row>
     <row r="165" spans="1:4">
       <c r="A165" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B165" s="2">
         <v>0.41</v>
       </c>
       <c r="C165" s="2">
-        <v>1.54</v>
+        <v>0</v>
       </c>
       <c r="D165" s="2">
         <v>1.95</v>
@@ -6222,13 +6216,13 @@
     </row>
     <row r="166" spans="1:4">
       <c r="A166" s="2" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="B166" s="2">
         <v>0.27</v>
       </c>
       <c r="C166" s="2">
-        <v>1.54</v>
+        <v>0</v>
       </c>
       <c r="D166" s="2">
         <v>1.81</v>
@@ -6236,13 +6230,13 @@
     </row>
     <row r="167" spans="1:4">
       <c r="A167" s="2" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="B167" s="2">
         <v>1.21</v>
       </c>
       <c r="C167" s="2">
-        <v>1.54</v>
+        <v>0</v>
       </c>
       <c r="D167" s="2">
         <v>2.75</v>
@@ -6255,7 +6249,7 @@
       </c>
       <c r="C168" s="3">
         <f t="shared" ref="C168:D168" si="21">AVERAGE(C162:C167)</f>
-        <v>1.54</v>
+        <v>0</v>
       </c>
       <c r="D168" s="3">
         <f t="shared" si="21"/>
@@ -6271,21 +6265,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100AEDD2C58C424B74499DE9AAA38D1F837" ma:contentTypeVersion="4" ma:contentTypeDescription="Opret et nyt dokument." ma:contentTypeScope="" ma:versionID="702f087d0813d5dfa38d019e1cfe3dbe">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="59a1f2c9-9aa0-4700-bb29-973d29195b9e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="6f1c68433e2c2319791049a96af9fb53" ns2:_="">
     <xsd:import namespace="59a1f2c9-9aa0-4700-bb29-973d29195b9e"/>
@@ -6429,14 +6408,29 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{80DA1591-5D0E-493F-827A-BF7F96FE3311}"/>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{540BE6A0-27F9-419F-8224-019FE94C5CBE}"/>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1B71B140-D529-43D3-80C5-DF1F266F3D83}"/>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{80DA1591-5D0E-493F-827A-BF7F96FE3311}"/>
 </file>
</xml_diff>